<commit_message>
Ajuste de hora de estudio por motivo imprevisto
</commit_message>
<xml_diff>
--- a/AGENDA 2023.xlsx
+++ b/AGENDA 2023.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desconocido7\Documents\Programando\Programando\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7E04942-2B64-41E7-8B43-79C4458B5079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC595C1-B7B6-4F10-92B2-8DC1D7E8D1FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="52">
   <si>
     <t>NOTAS</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>06/03/2023 - 12/03/2023</t>
+  </si>
+  <si>
+    <t>Estudiar informatica</t>
   </si>
 </sst>
 </file>
@@ -579,6 +582,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -589,7 +593,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,8 +813,8 @@
   </sheetPr>
   <dimension ref="A1:J953"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:B36"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="J86" sqref="J86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -831,16 +834,16 @@
     </row>
     <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="2"/>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="43" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="2:10" ht="21" x14ac:dyDescent="0.4">
       <c r="B3" s="3"/>
@@ -881,7 +884,7 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="11" t="s">
@@ -910,7 +913,7 @@
       </c>
     </row>
     <row r="6" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B6" s="46"/>
+      <c r="B6" s="47"/>
       <c r="C6" s="14" t="s">
         <v>10</v>
       </c>
@@ -923,7 +926,7 @@
       <c r="J6" s="16"/>
     </row>
     <row r="7" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B7" s="46"/>
+      <c r="B7" s="47"/>
       <c r="C7" s="17" t="s">
         <v>11</v>
       </c>
@@ -940,7 +943,7 @@
       <c r="J7" s="18"/>
     </row>
     <row r="8" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B8" s="46"/>
+      <c r="B8" s="47"/>
       <c r="C8" s="21" t="s">
         <v>14</v>
       </c>
@@ -957,7 +960,7 @@
       <c r="J8" s="22"/>
     </row>
     <row r="9" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B9" s="46"/>
+      <c r="B9" s="47"/>
       <c r="C9" s="23" t="s">
         <v>15</v>
       </c>
@@ -976,7 +979,7 @@
       <c r="J9" s="18"/>
     </row>
     <row r="10" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B10" s="46"/>
+      <c r="B10" s="47"/>
       <c r="C10" s="21" t="s">
         <v>19</v>
       </c>
@@ -997,7 +1000,7 @@
       <c r="J10" s="22"/>
     </row>
     <row r="11" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B11" s="46"/>
+      <c r="B11" s="47"/>
       <c r="C11" s="23" t="s">
         <v>21</v>
       </c>
@@ -1012,7 +1015,7 @@
       <c r="J11" s="18"/>
     </row>
     <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="47"/>
+      <c r="B12" s="48"/>
       <c r="C12" s="26" t="s">
         <v>23</v>
       </c>
@@ -1027,7 +1030,7 @@
       </c>
     </row>
     <row r="13" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="46" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="23" t="s">
@@ -1052,7 +1055,7 @@
       <c r="J13" s="32"/>
     </row>
     <row r="14" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B14" s="46"/>
+      <c r="B14" s="47"/>
       <c r="C14" s="21" t="s">
         <v>30</v>
       </c>
@@ -1075,7 +1078,7 @@
       <c r="J14" s="22"/>
     </row>
     <row r="15" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B15" s="46"/>
+      <c r="B15" s="47"/>
       <c r="C15" s="23" t="s">
         <v>31</v>
       </c>
@@ -1100,7 +1103,7 @@
       <c r="J15" s="18"/>
     </row>
     <row r="16" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B16" s="46"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="21" t="s">
         <v>35</v>
       </c>
@@ -1125,7 +1128,7 @@
       <c r="J16" s="22"/>
     </row>
     <row r="17" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B17" s="46"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="23" t="s">
         <v>37</v>
       </c>
@@ -1150,7 +1153,7 @@
       <c r="J17" s="18"/>
     </row>
     <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="47"/>
+      <c r="B18" s="48"/>
       <c r="C18" s="26" t="s">
         <v>39</v>
       </c>
@@ -1171,7 +1174,7 @@
       <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="46" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="23" t="s">
@@ -1194,7 +1197,7 @@
       <c r="J19" s="18"/>
     </row>
     <row r="20" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B20" s="46"/>
+      <c r="B20" s="47"/>
       <c r="C20" s="21" t="s">
         <v>44</v>
       </c>
@@ -1209,7 +1212,7 @@
       <c r="J20" s="22"/>
     </row>
     <row r="21" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B21" s="46"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="23" t="s">
         <v>45</v>
       </c>
@@ -1224,7 +1227,7 @@
       <c r="J21" s="18"/>
     </row>
     <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="46"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="26" t="s">
         <v>46</v>
       </c>
@@ -1237,7 +1240,7 @@
       <c r="J22" s="27"/>
     </row>
     <row r="23" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="47"/>
+      <c r="B23" s="48"/>
       <c r="C23" s="40">
         <v>0.91666666666666663</v>
       </c>
@@ -1256,21 +1259,21 @@
       <c r="B25" s="1"/>
     </row>
     <row r="26" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A26" s="48"/>
+      <c r="A26" s="42"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="43"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="44"/>
+      <c r="D26" s="44"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="45"/>
     </row>
     <row r="27" spans="1:10" ht="21" x14ac:dyDescent="0.4">
-      <c r="A27" s="48"/>
+      <c r="A27" s="42"/>
       <c r="B27" s="3"/>
       <c r="C27" s="4" t="s">
         <v>0</v>
@@ -1284,7 +1287,7 @@
       <c r="J27" s="5"/>
     </row>
     <row r="28" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="48"/>
+      <c r="A28" s="42"/>
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
       <c r="D28" s="10">
@@ -1310,8 +1313,8 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="48"/>
-      <c r="B29" s="45" t="s">
+      <c r="A29" s="42"/>
+      <c r="B29" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C29" s="11" t="s">
@@ -1340,8 +1343,8 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="48"/>
-      <c r="B30" s="46"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="14" t="s">
         <v>10</v>
       </c>
@@ -1354,8 +1357,8 @@
       <c r="J30" s="16"/>
     </row>
     <row r="31" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="48"/>
-      <c r="B31" s="46"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="47"/>
       <c r="C31" s="17" t="s">
         <v>11</v>
       </c>
@@ -1374,8 +1377,8 @@
       <c r="J31" s="18"/>
     </row>
     <row r="32" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="48"/>
-      <c r="B32" s="46"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="47"/>
       <c r="C32" s="21" t="s">
         <v>14</v>
       </c>
@@ -1394,8 +1397,8 @@
       <c r="J32" s="22"/>
     </row>
     <row r="33" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="48"/>
-      <c r="B33" s="46"/>
+      <c r="A33" s="42"/>
+      <c r="B33" s="47"/>
       <c r="C33" s="23" t="s">
         <v>15</v>
       </c>
@@ -1414,8 +1417,8 @@
       <c r="J33" s="18"/>
     </row>
     <row r="34" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="48"/>
-      <c r="B34" s="46"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="47"/>
       <c r="C34" s="21" t="s">
         <v>19</v>
       </c>
@@ -1436,8 +1439,8 @@
       <c r="J34" s="22"/>
     </row>
     <row r="35" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="48"/>
-      <c r="B35" s="46"/>
+      <c r="A35" s="42"/>
+      <c r="B35" s="47"/>
       <c r="C35" s="23" t="s">
         <v>21</v>
       </c>
@@ -1452,8 +1455,8 @@
       <c r="J35" s="18"/>
     </row>
     <row r="36" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="48"/>
-      <c r="B36" s="47"/>
+      <c r="A36" s="42"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="26" t="s">
         <v>23</v>
       </c>
@@ -1468,8 +1471,8 @@
       </c>
     </row>
     <row r="37" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="48"/>
-      <c r="B37" s="45" t="s">
+      <c r="A37" s="42"/>
+      <c r="B37" s="46" t="s">
         <v>25</v>
       </c>
       <c r="C37" s="23" t="s">
@@ -1494,8 +1497,8 @@
       <c r="J37" s="32"/>
     </row>
     <row r="38" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="48"/>
-      <c r="B38" s="46"/>
+      <c r="A38" s="42"/>
+      <c r="B38" s="47"/>
       <c r="C38" s="21" t="s">
         <v>30</v>
       </c>
@@ -1518,8 +1521,8 @@
       <c r="J38" s="22"/>
     </row>
     <row r="39" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A39" s="48"/>
-      <c r="B39" s="46"/>
+      <c r="A39" s="42"/>
+      <c r="B39" s="47"/>
       <c r="C39" s="23" t="s">
         <v>31</v>
       </c>
@@ -1544,8 +1547,8 @@
       <c r="J39" s="18"/>
     </row>
     <row r="40" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="48"/>
-      <c r="B40" s="46"/>
+      <c r="A40" s="42"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="21" t="s">
         <v>35</v>
       </c>
@@ -1570,8 +1573,8 @@
       <c r="J40" s="22"/>
     </row>
     <row r="41" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="48"/>
-      <c r="B41" s="46"/>
+      <c r="A41" s="42"/>
+      <c r="B41" s="47"/>
       <c r="C41" s="23" t="s">
         <v>37</v>
       </c>
@@ -1596,8 +1599,8 @@
       <c r="J41" s="18"/>
     </row>
     <row r="42" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="48"/>
-      <c r="B42" s="47"/>
+      <c r="A42" s="42"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="26" t="s">
         <v>39</v>
       </c>
@@ -1618,8 +1621,8 @@
       <c r="J42" s="27"/>
     </row>
     <row r="43" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="48"/>
-      <c r="B43" s="45" t="s">
+      <c r="A43" s="42"/>
+      <c r="B43" s="46" t="s">
         <v>41</v>
       </c>
       <c r="C43" s="23" t="s">
@@ -1642,8 +1645,8 @@
       <c r="J43" s="18"/>
     </row>
     <row r="44" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="48"/>
-      <c r="B44" s="46"/>
+      <c r="A44" s="42"/>
+      <c r="B44" s="47"/>
       <c r="C44" s="21" t="s">
         <v>44</v>
       </c>
@@ -1658,8 +1661,8 @@
       <c r="J44" s="22"/>
     </row>
     <row r="45" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="48"/>
-      <c r="B45" s="46"/>
+      <c r="A45" s="42"/>
+      <c r="B45" s="47"/>
       <c r="C45" s="23" t="s">
         <v>45</v>
       </c>
@@ -1674,8 +1677,8 @@
       <c r="J45" s="18"/>
     </row>
     <row r="46" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="48"/>
-      <c r="B46" s="46"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="47"/>
       <c r="C46" s="26" t="s">
         <v>46</v>
       </c>
@@ -1688,8 +1691,8 @@
       <c r="J46" s="27"/>
     </row>
     <row r="47" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="48"/>
-      <c r="B47" s="47"/>
+      <c r="A47" s="42"/>
+      <c r="B47" s="48"/>
       <c r="C47" s="40">
         <v>0.91666666666666663</v>
       </c>
@@ -1709,16 +1712,16 @@
     </row>
     <row r="50" spans="2:10" ht="21" x14ac:dyDescent="0.4">
       <c r="B50" s="2"/>
-      <c r="C50" s="42" t="s">
+      <c r="C50" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="43"/>
-      <c r="H50" s="43"/>
-      <c r="I50" s="43"/>
-      <c r="J50" s="44"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
+      <c r="F50" s="44"/>
+      <c r="G50" s="44"/>
+      <c r="H50" s="44"/>
+      <c r="I50" s="44"/>
+      <c r="J50" s="45"/>
     </row>
     <row r="51" spans="2:10" ht="21" x14ac:dyDescent="0.4">
       <c r="B51" s="3"/>
@@ -1759,7 +1762,7 @@
       </c>
     </row>
     <row r="53" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="45" t="s">
+      <c r="B53" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C53" s="11" t="s">
@@ -1788,7 +1791,7 @@
       </c>
     </row>
     <row r="54" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B54" s="46"/>
+      <c r="B54" s="47"/>
       <c r="C54" s="14" t="s">
         <v>10</v>
       </c>
@@ -1801,7 +1804,7 @@
       <c r="J54" s="16"/>
     </row>
     <row r="55" spans="2:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="46"/>
+      <c r="B55" s="47"/>
       <c r="C55" s="17" t="s">
         <v>11</v>
       </c>
@@ -1820,7 +1823,7 @@
       <c r="J55" s="18"/>
     </row>
     <row r="56" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B56" s="46"/>
+      <c r="B56" s="47"/>
       <c r="C56" s="21" t="s">
         <v>14</v>
       </c>
@@ -1839,7 +1842,7 @@
       <c r="J56" s="22"/>
     </row>
     <row r="57" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B57" s="46"/>
+      <c r="B57" s="47"/>
       <c r="C57" s="23" t="s">
         <v>15</v>
       </c>
@@ -1858,7 +1861,7 @@
       <c r="J57" s="18"/>
     </row>
     <row r="58" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B58" s="46"/>
+      <c r="B58" s="47"/>
       <c r="C58" s="21" t="s">
         <v>19</v>
       </c>
@@ -1879,7 +1882,7 @@
       <c r="J58" s="22"/>
     </row>
     <row r="59" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B59" s="46"/>
+      <c r="B59" s="47"/>
       <c r="C59" s="23" t="s">
         <v>21</v>
       </c>
@@ -1894,7 +1897,7 @@
       <c r="J59" s="18"/>
     </row>
     <row r="60" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B60" s="47"/>
+      <c r="B60" s="48"/>
       <c r="C60" s="26" t="s">
         <v>23</v>
       </c>
@@ -1909,7 +1912,7 @@
       </c>
     </row>
     <row r="61" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="45" t="s">
+      <c r="B61" s="46" t="s">
         <v>25</v>
       </c>
       <c r="C61" s="23" t="s">
@@ -1934,7 +1937,7 @@
       <c r="J61" s="32"/>
     </row>
     <row r="62" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B62" s="46"/>
+      <c r="B62" s="47"/>
       <c r="C62" s="21" t="s">
         <v>30</v>
       </c>
@@ -1957,7 +1960,7 @@
       <c r="J62" s="22"/>
     </row>
     <row r="63" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B63" s="46"/>
+      <c r="B63" s="47"/>
       <c r="C63" s="23" t="s">
         <v>31</v>
       </c>
@@ -1982,7 +1985,7 @@
       <c r="J63" s="18"/>
     </row>
     <row r="64" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B64" s="46"/>
+      <c r="B64" s="47"/>
       <c r="C64" s="21" t="s">
         <v>35</v>
       </c>
@@ -2007,7 +2010,7 @@
       <c r="J64" s="22"/>
     </row>
     <row r="65" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B65" s="46"/>
+      <c r="B65" s="47"/>
       <c r="C65" s="23" t="s">
         <v>37</v>
       </c>
@@ -2032,7 +2035,7 @@
       <c r="J65" s="18"/>
     </row>
     <row r="66" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="47"/>
+      <c r="B66" s="48"/>
       <c r="C66" s="26" t="s">
         <v>39</v>
       </c>
@@ -2053,7 +2056,7 @@
       <c r="J66" s="27"/>
     </row>
     <row r="67" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="45" t="s">
+      <c r="B67" s="46" t="s">
         <v>41</v>
       </c>
       <c r="C67" s="23" t="s">
@@ -2076,7 +2079,7 @@
       <c r="J67" s="18"/>
     </row>
     <row r="68" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B68" s="46"/>
+      <c r="B68" s="47"/>
       <c r="C68" s="21" t="s">
         <v>44</v>
       </c>
@@ -2091,7 +2094,7 @@
       <c r="J68" s="22"/>
     </row>
     <row r="69" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B69" s="46"/>
+      <c r="B69" s="47"/>
       <c r="C69" s="23" t="s">
         <v>45</v>
       </c>
@@ -2106,7 +2109,7 @@
       <c r="J69" s="18"/>
     </row>
     <row r="70" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B70" s="46"/>
+      <c r="B70" s="47"/>
       <c r="C70" s="26" t="s">
         <v>46</v>
       </c>
@@ -2119,7 +2122,7 @@
       <c r="J70" s="27"/>
     </row>
     <row r="71" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="47"/>
+      <c r="B71" s="48"/>
       <c r="C71" s="40">
         <v>0.91666666666666663</v>
       </c>
@@ -2136,16 +2139,16 @@
     </row>
     <row r="73" spans="2:10" ht="21" x14ac:dyDescent="0.4">
       <c r="B73" s="2"/>
-      <c r="C73" s="42" t="s">
+      <c r="C73" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="D73" s="43"/>
-      <c r="E73" s="43"/>
-      <c r="F73" s="43"/>
-      <c r="G73" s="43"/>
-      <c r="H73" s="43"/>
-      <c r="I73" s="43"/>
-      <c r="J73" s="44"/>
+      <c r="D73" s="44"/>
+      <c r="E73" s="44"/>
+      <c r="F73" s="44"/>
+      <c r="G73" s="44"/>
+      <c r="H73" s="44"/>
+      <c r="I73" s="44"/>
+      <c r="J73" s="45"/>
     </row>
     <row r="74" spans="2:10" ht="21" x14ac:dyDescent="0.4">
       <c r="B74" s="3"/>
@@ -2186,7 +2189,7 @@
       </c>
     </row>
     <row r="76" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B76" s="45" t="s">
+      <c r="B76" s="46" t="s">
         <v>1</v>
       </c>
       <c r="C76" s="11" t="s">
@@ -2215,7 +2218,7 @@
       </c>
     </row>
     <row r="77" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B77" s="46"/>
+      <c r="B77" s="47"/>
       <c r="C77" s="14" t="s">
         <v>10</v>
       </c>
@@ -2228,7 +2231,7 @@
       <c r="J77" s="16"/>
     </row>
     <row r="78" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B78" s="46"/>
+      <c r="B78" s="47"/>
       <c r="C78" s="17" t="s">
         <v>11</v>
       </c>
@@ -2247,7 +2250,7 @@
       <c r="J78" s="18"/>
     </row>
     <row r="79" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B79" s="46"/>
+      <c r="B79" s="47"/>
       <c r="C79" s="21" t="s">
         <v>14</v>
       </c>
@@ -2266,7 +2269,7 @@
       <c r="J79" s="22"/>
     </row>
     <row r="80" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B80" s="46"/>
+      <c r="B80" s="47"/>
       <c r="C80" s="23" t="s">
         <v>15</v>
       </c>
@@ -2285,7 +2288,7 @@
       <c r="J80" s="18"/>
     </row>
     <row r="81" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B81" s="46"/>
+      <c r="B81" s="47"/>
       <c r="C81" s="21" t="s">
         <v>19</v>
       </c>
@@ -2306,7 +2309,7 @@
       <c r="J81" s="22"/>
     </row>
     <row r="82" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B82" s="46"/>
+      <c r="B82" s="47"/>
       <c r="C82" s="23" t="s">
         <v>21</v>
       </c>
@@ -2321,7 +2324,7 @@
       <c r="J82" s="18"/>
     </row>
     <row r="83" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B83" s="47"/>
+      <c r="B83" s="48"/>
       <c r="C83" s="26" t="s">
         <v>23</v>
       </c>
@@ -2336,7 +2339,7 @@
       </c>
     </row>
     <row r="84" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B84" s="45" t="s">
+      <c r="B84" s="46" t="s">
         <v>25</v>
       </c>
       <c r="C84" s="23" t="s">
@@ -2365,7 +2368,7 @@
       </c>
     </row>
     <row r="85" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B85" s="46"/>
+      <c r="B85" s="47"/>
       <c r="C85" s="21" t="s">
         <v>30</v>
       </c>
@@ -2392,7 +2395,7 @@
       </c>
     </row>
     <row r="86" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B86" s="46"/>
+      <c r="B86" s="47"/>
       <c r="C86" s="23" t="s">
         <v>31</v>
       </c>
@@ -2417,7 +2420,7 @@
       <c r="J86" s="18"/>
     </row>
     <row r="87" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B87" s="46"/>
+      <c r="B87" s="47"/>
       <c r="C87" s="21" t="s">
         <v>35</v>
       </c>
@@ -2442,7 +2445,7 @@
       <c r="J87" s="22"/>
     </row>
     <row r="88" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B88" s="46"/>
+      <c r="B88" s="47"/>
       <c r="C88" s="23" t="s">
         <v>37</v>
       </c>
@@ -2455,9 +2458,7 @@
       <c r="F88" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="G88" s="33" t="s">
-        <v>38</v>
-      </c>
+      <c r="G88" s="33"/>
       <c r="H88" s="37" t="s">
         <v>33</v>
       </c>
@@ -2467,7 +2468,7 @@
       <c r="J88" s="18"/>
     </row>
     <row r="89" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B89" s="47"/>
+      <c r="B89" s="48"/>
       <c r="C89" s="26" t="s">
         <v>39</v>
       </c>
@@ -2478,17 +2479,17 @@
         <v>38</v>
       </c>
       <c r="F89" s="27"/>
-      <c r="G89" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="H89" s="27"/>
+      <c r="G89" s="38"/>
+      <c r="H89" s="27" t="s">
+        <v>51</v>
+      </c>
       <c r="I89" s="27" t="s">
         <v>40</v>
       </c>
       <c r="J89" s="27"/>
     </row>
     <row r="90" spans="2:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="45" t="s">
+      <c r="B90" s="46" t="s">
         <v>41</v>
       </c>
       <c r="C90" s="23" t="s">
@@ -2502,31 +2503,37 @@
       </c>
       <c r="F90" s="18"/>
       <c r="G90" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="H90" s="18"/>
+        <v>33</v>
+      </c>
+      <c r="H90" s="18" t="s">
+        <v>51</v>
+      </c>
       <c r="I90" s="32" t="s">
         <v>40</v>
       </c>
       <c r="J90" s="18"/>
     </row>
     <row r="91" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B91" s="46"/>
+      <c r="B91" s="47"/>
       <c r="C91" s="21" t="s">
         <v>44</v>
       </c>
       <c r="D91" s="22"/>
       <c r="E91" s="22"/>
       <c r="F91" s="22"/>
-      <c r="G91" s="22"/>
-      <c r="H91" s="22"/>
+      <c r="G91" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="H91" s="22" t="s">
+        <v>51</v>
+      </c>
       <c r="I91" s="39" t="s">
         <v>40</v>
       </c>
       <c r="J91" s="22"/>
     </row>
     <row r="92" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B92" s="46"/>
+      <c r="B92" s="47"/>
       <c r="C92" s="23" t="s">
         <v>45</v>
       </c>
@@ -2541,7 +2548,7 @@
       <c r="J92" s="18"/>
     </row>
     <row r="93" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B93" s="46"/>
+      <c r="B93" s="47"/>
       <c r="C93" s="26" t="s">
         <v>46</v>
       </c>
@@ -2554,7 +2561,7 @@
       <c r="J93" s="27"/>
     </row>
     <row r="94" spans="2:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B94" s="47"/>
+      <c r="B94" s="48"/>
       <c r="C94" s="40">
         <v>0.91666666666666663</v>
       </c>
@@ -5095,22 +5102,22 @@
     <row r="953" ht="13.2" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C26:J26"/>
-    <mergeCell ref="B29:B36"/>
-    <mergeCell ref="B37:B42"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="C50:J50"/>
+    <mergeCell ref="C73:J73"/>
+    <mergeCell ref="B76:B83"/>
+    <mergeCell ref="B84:B89"/>
+    <mergeCell ref="B90:B94"/>
+    <mergeCell ref="C2:J2"/>
     <mergeCell ref="B5:B12"/>
     <mergeCell ref="B13:B18"/>
     <mergeCell ref="B61:B66"/>
     <mergeCell ref="B67:B71"/>
     <mergeCell ref="B19:B23"/>
     <mergeCell ref="B53:B60"/>
-    <mergeCell ref="C73:J73"/>
-    <mergeCell ref="B76:B83"/>
-    <mergeCell ref="B84:B89"/>
-    <mergeCell ref="B90:B94"/>
-    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C26:J26"/>
+    <mergeCell ref="B29:B36"/>
+    <mergeCell ref="B37:B42"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="C50:J50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>